<commit_message>
Add FastAPI target API + Docker/Compose + CI trigger + stabilize test runner
</commit_message>
<xml_diff>
--- a/database/DemoAPITestCase.xlsx
+++ b/database/DemoAPITestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivianbb/Downloads/APITest-public/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0C99E9-8E59-304D-B6C4-B18806FC6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1CAD2B-A9F5-D540-9ED1-F38F2697F6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="760" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>event_query_001</t>
   </si>
   <si>
-    <t>http://127.0.0.1:8000/api/get_event_list/</t>
-  </si>
-  <si>
     <t>get</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>quest_query_011</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:8000/api/get_guest_list/</t>
   </si>
   <si>
     <t>quest_query_012</t>
@@ -310,12 +304,18 @@
   <si>
     <t>{"eid":1,"phone":13355556666}</t>
   </si>
+  <si>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/get_event_list/	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://127.0.0.1:8000/api/get_guest_list/	</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +379,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -418,12 +427,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -464,8 +476,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,9 +789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -780,7 +799,7 @@
     <col min="1" max="1" width="10.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="36" style="3" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="61.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" style="3" customWidth="1"/>
@@ -793,63 +812,63 @@
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -858,29 +877,29 @@
         <v>200</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" ht="30" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -889,29 +908,29 @@
         <v>200</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>5</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -920,29 +939,29 @@
         <v>10021</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="F5" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -951,29 +970,29 @@
         <v>10022</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="F6" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -982,204 +1001,204 @@
         <v>10022</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="43.5" customHeight="1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="55.5" customHeight="1">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="57" customHeight="1">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="11">
         <v>10023</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" ht="52.5" customHeight="1">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J10" s="11">
         <v>10024</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="51.75" customHeight="1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J11" s="11">
         <v>200</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="35.25" customHeight="1">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1188,29 +1207,29 @@
         <v>200</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>16</v>
+        <v>65</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1219,29 +1238,29 @@
         <v>200</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>16</v>
+        <v>66</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1250,29 +1269,29 @@
         <v>10021</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>16</v>
+        <v>67</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1281,29 +1300,29 @@
         <v>10022</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="26.25" customHeight="1">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>16</v>
+        <v>68</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1312,7 +1331,7 @@
         <v>10022</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1406,21 +1425,21 @@
   <autoFilter ref="A1:M15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D6" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D5" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D3" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{A879422A-FA34-0943-9180-5109853F45A9}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{48DC90D3-BE12-EF4C-B0AF-1F0B7816C96D}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{64AC5816-5817-A342-9011-4CEE437B2661}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{BE1D384E-0C28-7543-8A37-F48DD725B295}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{42A3035B-7188-1C43-B9DA-4DC3B0B4AED0}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{F3AFCCB4-4C18-1743-8FBE-09AA2842BBF3}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{FA21A15A-8E64-8243-8AAF-4ADDB2E788D8}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{3C729436-D150-2E4E-8D87-A3121A8FE319}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{F37E6D9D-199E-BE4F-A9B9-A96DFFC865A4}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{EE2C399F-68BD-AE4D-A566-29367C75BB98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>

</xml_diff>